<commit_message>
deleted:    Exam Timetable.xlsx 	modified:   Input/2122 1st/Exam Timetable.xlsx 	modified:   Input/2122 2nd/Exam Timetable.xlsx 	modified:   Input/2122 final/Exam Timetable.xlsx 	modified:   Input/2122 final/Other Info.xlsx 	deleted:    Input/Exam Timetable.xlsx 	deleted:    Input/Other Info.xlsx 	deleted:    Input/Specific Examer.xlsx 	deleted:    Input/Teacher Timetable.xlsx 	modified:   function_set.py 	modified:   main.ipynb 	modified:   main.py 	modified:   try.ipynb 	modified:   "\347\233\243\350\200\203\346\231\202\351\226\223\350\241\250.xlsx"
</commit_message>
<xml_diff>
--- a/Input/2122 1st/Exam Timetable.xlsx
+++ b/Input/2122 1st/Exam Timetable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio Code Projects\TSTSS_Exam_Timetable\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Visual Studio Code Projects\TSTSS_Exam_Timetable\Input\2122 1st\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EC6EC9-2DAB-441E-9120-1EDBAD6CAC89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB23F82-5A9C-4F73-B3C9-52C8CE3BC650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3360" yWindow="3360" windowWidth="18514" windowHeight="10834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="174">
   <si>
     <t>科    目</t>
   </si>
@@ -322,21 +322,6 @@
   </si>
   <si>
     <t>301, 302, 601, 602</t>
-  </si>
-  <si>
-    <t>301, 302, 601, 603</t>
-  </si>
-  <si>
-    <t>301, 302, 601, 604</t>
-  </si>
-  <si>
-    <t>301, 302, 601, 605</t>
-  </si>
-  <si>
-    <t>301, 302, 601, 606</t>
-  </si>
-  <si>
-    <t>301, 302, 601, 607</t>
   </si>
   <si>
     <t>綜合人文
@@ -866,7 +851,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -921,6 +906,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1214,16 +1202,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="11" width="16.625" customWidth="1"/>
+    <col min="2" max="11" width="16.640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
@@ -1238,7 +1226,7 @@
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="10"/>
       <c r="B2" s="11" t="s">
         <v>14</v>
@@ -1262,17 +1250,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="20" t="s">
         <v>22</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -1288,13 +1276,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
       <c r="E4" s="6">
         <v>60</v>
       </c>
@@ -1308,13 +1296,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
       <c r="E5" s="6" t="s">
         <v>23</v>
       </c>
@@ -1328,13 +1316,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="7" t="s">
         <v>24</v>
       </c>
@@ -1348,17 +1336,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="20" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -1374,13 +1362,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
       <c r="E8" s="6">
         <v>60</v>
       </c>
@@ -1394,13 +1382,13 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="6" t="s">
         <v>23</v>
       </c>
@@ -1414,13 +1402,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="7" t="s">
         <v>32</v>
       </c>
@@ -1434,17 +1422,17 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="20" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -1454,49 +1442,49 @@
       <c r="G11" s="19"/>
       <c r="H11" s="19"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
       <c r="E12" s="6">
         <v>30</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
       <c r="E13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-    </row>
-    <row r="14" spans="1:11" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
       <c r="E14" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="15"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
@@ -1506,7 +1494,7 @@
       <c r="G15" s="15"/>
       <c r="H15" s="15"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="15" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
         <v>4</v>
       </c>
@@ -1518,7 +1506,7 @@
       <c r="G16" s="15"/>
       <c r="H16" s="15"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A17" s="2"/>
       <c r="B17" s="11" t="str">
         <f t="shared" ref="B17:H17" si="0">B2</f>
@@ -1549,17 +1537,17 @@
         <v>12/11/2021 (五)</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="20" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -1575,13 +1563,13 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
       <c r="E19" s="6">
         <v>60</v>
       </c>
@@ -1595,13 +1583,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
       <c r="E20" s="6" t="s">
         <v>39</v>
       </c>
@@ -1615,13 +1603,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
       <c r="E21" s="7" t="s">
         <v>24</v>
       </c>
@@ -1635,24 +1623,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="20" t="s">
         <v>22</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>43</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>44</v>
@@ -1661,13 +1649,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
       <c r="E23" s="6">
         <v>75</v>
       </c>
@@ -1681,13 +1669,13 @@
         <v>75</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
       <c r="E24" s="6" t="s">
         <v>39</v>
       </c>
@@ -1701,13 +1689,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
       <c r="E25" s="7" t="s">
         <v>33</v>
       </c>
@@ -1715,23 +1703,23 @@
         <v>33</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="20" t="s">
         <v>22</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -1741,49 +1729,49 @@
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
     </row>
-    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
       <c r="E27" s="6">
         <v>30</v>
       </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-    </row>
-    <row r="28" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+    </row>
+    <row r="28" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
       <c r="E28" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20"/>
-    </row>
-    <row r="29" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+    </row>
+    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
       <c r="E29" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="15"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -1793,7 +1781,7 @@
       <c r="G30" s="15"/>
       <c r="H30" s="15"/>
     </row>
-    <row r="31" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A31" s="16" t="s">
         <v>5</v>
       </c>
@@ -1805,7 +1793,7 @@
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
     </row>
-    <row r="32" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A32" s="2"/>
       <c r="B32" s="11" t="str">
         <f t="shared" ref="B32:H32" si="1">B2</f>
@@ -1836,7 +1824,7 @@
         <v>12/11/2021 (五)</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>10</v>
       </c>
@@ -1860,7 +1848,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>11</v>
       </c>
@@ -1879,12 +1867,12 @@
       <c r="F34" s="6">
         <v>60</v>
       </c>
-      <c r="G34" s="20"/>
+      <c r="G34" s="19"/>
       <c r="H34" s="6">
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>12</v>
       </c>
@@ -1895,20 +1883,20 @@
         <v>61</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="G35" s="20"/>
+        <v>61</v>
+      </c>
+      <c r="G35" s="19"/>
       <c r="H35" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>9</v>
       </c>
@@ -1916,10 +1904,10 @@
         <v>24</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E36" s="7" t="s">
         <v>24</v>
@@ -1927,12 +1915,12 @@
       <c r="F36" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G36" s="21"/>
+      <c r="G36" s="19"/>
       <c r="H36" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>10</v>
       </c>
@@ -1956,7 +1944,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>11</v>
       </c>
@@ -1975,12 +1963,12 @@
       <c r="F38" s="6">
         <v>30</v>
       </c>
-      <c r="G38" s="20"/>
+      <c r="G38" s="19"/>
       <c r="H38" s="6">
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>12</v>
       </c>
@@ -1988,47 +1976,47 @@
         <v>61</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D39" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G39" s="19"/>
+      <c r="H39" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="G39" s="20"/>
-      <c r="H39" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="G40" s="21"/>
+        <v>66</v>
+      </c>
+      <c r="G40" s="19"/>
       <c r="H40" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>13</v>
       </c>
@@ -2042,49 +2030,49 @@
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
       <c r="H42" s="6">
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
       <c r="H43" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
       <c r="H44" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="15"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
@@ -2094,7 +2082,7 @@
       <c r="G45" s="15"/>
       <c r="H45" s="15"/>
     </row>
-    <row r="46" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A46" s="17" t="s">
         <v>6</v>
       </c>
@@ -2106,7 +2094,7 @@
       <c r="G46" s="15"/>
       <c r="H46" s="15"/>
     </row>
-    <row r="47" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A47" s="2"/>
       <c r="B47" s="11" t="str">
         <f t="shared" ref="B47:H47" si="2">B2</f>
@@ -2137,33 +2125,33 @@
         <v>12/11/2021 (五)</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="57" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" ht="56.6" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F48" s="5" t="s">
         <v>58</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>11</v>
       </c>
@@ -2189,38 +2177,38 @@
         <v>90</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>31</v>
@@ -2232,33 +2220,33 @@
         <v>31</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>50</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>59</v>
@@ -2267,7 +2255,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>11</v>
       </c>
@@ -2293,47 +2281,47 @@
         <v>90</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A54" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C54" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H54" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="D54" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H54" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F55" s="7" t="s">
         <v>31</v>
@@ -2342,10 +2330,10 @@
         <v>24</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>13</v>
       </c>
@@ -2353,23 +2341,23 @@
       <c r="C56" s="19"/>
       <c r="D56" s="19"/>
       <c r="E56" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="H56" s="19"/>
     </row>
-    <row r="57" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
       <c r="E57" s="6">
         <v>90</v>
       </c>
@@ -2379,45 +2367,45 @@
       <c r="G57" s="6">
         <v>90</v>
       </c>
-      <c r="H57" s="20"/>
-    </row>
-    <row r="58" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="H57" s="19"/>
+    </row>
+    <row r="58" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
       <c r="E58" s="6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="H58" s="20"/>
-    </row>
-    <row r="59" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="H58" s="19"/>
+    </row>
+    <row r="59" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B59" s="21"/>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19"/>
       <c r="E59" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G59" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="H59" s="21"/>
-    </row>
-    <row r="60" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="H59" s="19"/>
+    </row>
+    <row r="60" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>13</v>
       </c>
@@ -2426,54 +2414,54 @@
       <c r="D60" s="19"/>
       <c r="E60" s="19"/>
       <c r="F60" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G60" s="19"/>
       <c r="H60" s="19"/>
     </row>
-    <row r="61" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B61" s="20"/>
-      <c r="C61" s="20"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
       <c r="F61" s="6">
         <v>60</v>
       </c>
-      <c r="G61" s="20"/>
-      <c r="H61" s="20"/>
-    </row>
-    <row r="62" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="G61" s="19"/>
+      <c r="H61" s="19"/>
+    </row>
+    <row r="62" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B62" s="20"/>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="19"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
       <c r="F62" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="G62" s="20"/>
-      <c r="H62" s="20"/>
-    </row>
-    <row r="63" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+      <c r="G62" s="19"/>
+      <c r="H62" s="19"/>
+    </row>
+    <row r="63" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B63" s="21"/>
-      <c r="C63" s="21"/>
-      <c r="D63" s="21"/>
-      <c r="E63" s="21"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
       <c r="F63" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G63" s="21"/>
-      <c r="H63" s="21"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G63" s="19"/>
+      <c r="H63" s="19"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="15"/>
       <c r="B64" s="15"/>
       <c r="C64" s="15"/>
@@ -2483,7 +2471,7 @@
       <c r="G64" s="15"/>
       <c r="H64" s="15"/>
     </row>
-    <row r="65" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A65" s="17" t="s">
         <v>7</v>
       </c>
@@ -2495,7 +2483,7 @@
       <c r="G65" s="15"/>
       <c r="H65" s="15"/>
     </row>
-    <row r="66" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A66" s="2"/>
       <c r="B66" s="11" t="str">
         <f t="shared" ref="B66:H66" si="3">B2</f>
@@ -2526,33 +2514,33 @@
         <v>12/11/2021 (五)</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" ht="42.45" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>59</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
         <v>11</v>
       </c>
@@ -2578,33 +2566,33 @@
         <v>180</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>9</v>
       </c>
@@ -2618,7 +2606,7 @@
         <v>31</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F70" s="7" t="s">
         <v>31</v>
@@ -2627,34 +2615,34 @@
         <v>31</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G71" s="18"/>
       <c r="H71" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
         <v>11</v>
       </c>
@@ -2678,71 +2666,71 @@
         <v>55</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B73" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D73" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C73" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>119</v>
-      </c>
       <c r="E73" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G73" s="18"/>
       <c r="H73" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C74" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>31</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G74" s="18"/>
       <c r="H74" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B75" s="18"/>
       <c r="C75" s="18"/>
       <c r="D75" s="5" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E75" s="18"/>
       <c r="F75" s="18"/>
       <c r="G75" s="18"/>
       <c r="H75" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
         <v>11</v>
       </c>
@@ -2758,23 +2746,23 @@
         <v>90</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B77" s="18"/>
       <c r="C77" s="18"/>
       <c r="D77" s="6" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E77" s="18"/>
       <c r="F77" s="18"/>
       <c r="G77" s="18"/>
       <c r="H77" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>9</v>
       </c>
@@ -2790,7 +2778,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>13</v>
       </c>
@@ -2803,10 +2791,10 @@
       <c r="F79" s="18"/>
       <c r="G79" s="18"/>
       <c r="H79" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
         <v>11</v>
       </c>
@@ -2822,55 +2810,55 @@
         <v>120</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B81" s="18"/>
       <c r="C81" s="18"/>
       <c r="D81" s="6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E81" s="18"/>
       <c r="F81" s="18"/>
       <c r="G81" s="18"/>
       <c r="H81" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B82" s="18"/>
       <c r="C82" s="18"/>
       <c r="D82" s="7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E82" s="18"/>
       <c r="F82" s="18"/>
       <c r="G82" s="18"/>
       <c r="H82" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B83" s="18"/>
       <c r="C83" s="18"/>
       <c r="D83" s="5" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E83" s="18"/>
       <c r="F83" s="18"/>
       <c r="G83" s="18"/>
       <c r="H83" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
         <v>11</v>
       </c>
@@ -2886,53 +2874,53 @@
         <v>120</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B85" s="18"/>
       <c r="C85" s="18"/>
       <c r="D85" s="6" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E85" s="18"/>
       <c r="F85" s="18"/>
       <c r="G85" s="18"/>
       <c r="H85" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B86" s="18"/>
       <c r="C86" s="18"/>
       <c r="D86" s="7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E86" s="18"/>
       <c r="F86" s="18"/>
       <c r="G86" s="18"/>
       <c r="H86" s="7" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B87" s="18"/>
       <c r="C87" s="18"/>
       <c r="D87" s="5" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E87" s="18"/>
       <c r="F87" s="18"/>
       <c r="G87" s="18"/>
       <c r="H87" s="18"/>
     </row>
-    <row r="88" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
         <v>11</v>
       </c>
@@ -2946,35 +2934,35 @@
       <c r="G88" s="18"/>
       <c r="H88" s="18"/>
     </row>
-    <row r="89" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B89" s="18"/>
       <c r="C89" s="18"/>
       <c r="D89" s="6" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="E89" s="18"/>
       <c r="F89" s="18"/>
       <c r="G89" s="18"/>
       <c r="H89" s="18"/>
     </row>
-    <row r="90" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B90" s="18"/>
       <c r="C90" s="18"/>
       <c r="D90" s="7" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E90" s="18"/>
       <c r="F90" s="18"/>
       <c r="G90" s="18"/>
       <c r="H90" s="18"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" s="15"/>
       <c r="B91" s="15"/>
       <c r="C91" s="15"/>
@@ -2984,7 +2972,7 @@
       <c r="G91" s="15"/>
       <c r="H91" s="15"/>
     </row>
-    <row r="92" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A92" s="17" t="s">
         <v>8</v>
       </c>
@@ -2996,7 +2984,7 @@
       <c r="G92" s="15"/>
       <c r="H92" s="15"/>
     </row>
-    <row r="93" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A93" s="2"/>
       <c r="B93" s="11" t="str">
         <f t="shared" ref="B93:H93" si="4">B2</f>
@@ -3027,33 +3015,33 @@
         <v>12/11/2021 (五)</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G94" s="5" t="s">
         <v>58</v>
       </c>
       <c r="H94" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="s">
         <v>11</v>
       </c>
@@ -3079,33 +3067,33 @@
         <v>135</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F96" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G96" s="6" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H96" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>9</v>
       </c>
@@ -3116,48 +3104,48 @@
         <v>31</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="F97" s="7" t="s">
         <v>31</v>
       </c>
       <c r="G97" s="7" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E98" s="5" t="s">
         <v>59</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H98" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
         <v>11</v>
       </c>
@@ -3183,379 +3171,378 @@
         <v>150</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F100" s="6" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="G100" s="6" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="H100" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C101" s="7" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="D101" s="7" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G101" s="7" t="s">
         <v>31</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B102" s="5"/>
-      <c r="C102" s="5"/>
-      <c r="D102" s="5"/>
+      <c r="B102" s="18"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="18"/>
       <c r="E102" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="F102" s="5"/>
+        <v>113</v>
+      </c>
+      <c r="F102" s="18"/>
       <c r="G102" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="H102" s="5"/>
-    </row>
-    <row r="103" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+      <c r="H102" s="18"/>
+    </row>
+    <row r="103" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A103" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B103" s="6"/>
-      <c r="C103" s="6"/>
-      <c r="D103" s="6"/>
+      <c r="B103" s="18"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="18"/>
       <c r="E103" s="6">
         <v>90</v>
       </c>
-      <c r="F103" s="6"/>
+      <c r="F103" s="18"/>
       <c r="G103" s="6">
         <v>75</v>
       </c>
-      <c r="H103" s="6"/>
-    </row>
-    <row r="104" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="H103" s="18"/>
+    </row>
+    <row r="104" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A104" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B104" s="6"/>
-      <c r="C104" s="6"/>
-      <c r="D104" s="6"/>
+      <c r="B104" s="18"/>
+      <c r="C104" s="18"/>
+      <c r="D104" s="18"/>
       <c r="E104" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="F104" s="6"/>
+        <v>167</v>
+      </c>
+      <c r="F104" s="18"/>
       <c r="G104" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="H104" s="6"/>
-    </row>
-    <row r="105" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+      <c r="H104" s="18"/>
+    </row>
+    <row r="105" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B105" s="7"/>
-      <c r="C105" s="7"/>
-      <c r="D105" s="7"/>
+      <c r="B105" s="18"/>
+      <c r="C105" s="18"/>
+      <c r="D105" s="18"/>
       <c r="E105" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F105" s="7"/>
+      <c r="F105" s="18"/>
       <c r="G105" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H105" s="7"/>
-    </row>
-    <row r="106" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="H105" s="18"/>
+    </row>
+    <row r="106" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B106" s="5"/>
-      <c r="C106" s="5"/>
-      <c r="D106" s="5"/>
+      <c r="B106" s="18"/>
+      <c r="C106" s="18"/>
+      <c r="D106" s="18"/>
       <c r="E106" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="F106" s="5"/>
+        <v>144</v>
+      </c>
+      <c r="F106" s="18"/>
       <c r="G106" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="H106" s="5"/>
-    </row>
-    <row r="107" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="H106" s="18"/>
+    </row>
+    <row r="107" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A107" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B107" s="6"/>
-      <c r="C107" s="6"/>
-      <c r="D107" s="6"/>
+      <c r="B107" s="18"/>
+      <c r="C107" s="18"/>
+      <c r="D107" s="18"/>
       <c r="E107" s="6">
         <v>60</v>
       </c>
-      <c r="F107" s="6"/>
+      <c r="F107" s="18"/>
       <c r="G107" s="6">
         <v>150</v>
       </c>
-      <c r="H107" s="6"/>
-    </row>
-    <row r="108" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="H107" s="18"/>
+    </row>
+    <row r="108" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A108" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B108" s="6"/>
-      <c r="C108" s="6"/>
-      <c r="D108" s="6"/>
+      <c r="B108" s="18"/>
+      <c r="C108" s="18"/>
+      <c r="D108" s="18"/>
       <c r="E108" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="F108" s="6"/>
+        <v>168</v>
+      </c>
+      <c r="F108" s="18"/>
       <c r="G108" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="H108" s="6"/>
-    </row>
-    <row r="109" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+      <c r="H108" s="18"/>
+    </row>
+    <row r="109" spans="1:8" ht="15" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B109" s="7"/>
-      <c r="C109" s="7"/>
-      <c r="D109" s="7"/>
+      <c r="B109" s="18"/>
+      <c r="C109" s="18"/>
+      <c r="D109" s="18"/>
       <c r="E109" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F109" s="7"/>
+      <c r="F109" s="18"/>
       <c r="G109" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="H109" s="7"/>
-    </row>
-    <row r="110" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+      <c r="H109" s="18"/>
+    </row>
+    <row r="110" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B110" s="5"/>
-      <c r="C110" s="5"/>
-      <c r="D110" s="5"/>
+      <c r="B110" s="18"/>
+      <c r="C110" s="18"/>
+      <c r="D110" s="18"/>
       <c r="E110" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F110" s="5"/>
+      <c r="F110" s="18"/>
       <c r="G110" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="H110" s="5"/>
-    </row>
-    <row r="111" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+      <c r="H110" s="18"/>
+    </row>
+    <row r="111" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A111" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B111" s="6"/>
-      <c r="C111" s="6"/>
-      <c r="D111" s="6"/>
+      <c r="B111" s="18"/>
+      <c r="C111" s="18"/>
+      <c r="D111" s="18"/>
       <c r="E111" s="6">
         <v>150</v>
       </c>
-      <c r="F111" s="6"/>
+      <c r="F111" s="18"/>
       <c r="G111" s="6">
         <v>60</v>
       </c>
-      <c r="H111" s="6"/>
-    </row>
-    <row r="112" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="H111" s="18"/>
+    </row>
+    <row r="112" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A112" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B112" s="6"/>
-      <c r="C112" s="6"/>
-      <c r="D112" s="6"/>
+      <c r="B112" s="18"/>
+      <c r="C112" s="18"/>
+      <c r="D112" s="18"/>
       <c r="E112" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="F112" s="6"/>
+        <v>169</v>
+      </c>
+      <c r="F112" s="18"/>
       <c r="G112" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="H112" s="6"/>
-    </row>
-    <row r="113" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+      <c r="H112" s="18"/>
+    </row>
+    <row r="113" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B113" s="7"/>
-      <c r="C113" s="7"/>
-      <c r="D113" s="7"/>
+      <c r="B113" s="18"/>
+      <c r="C113" s="18"/>
+      <c r="D113" s="18"/>
       <c r="E113" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="F113" s="7"/>
+        <v>153</v>
+      </c>
+      <c r="F113" s="18"/>
       <c r="G113" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="H113" s="7"/>
-    </row>
-    <row r="114" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+      <c r="H113" s="18"/>
+    </row>
+    <row r="114" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B114" s="5"/>
-      <c r="C114" s="5"/>
-      <c r="D114" s="5"/>
+      <c r="B114" s="18"/>
+      <c r="C114" s="18"/>
+      <c r="D114" s="18"/>
       <c r="E114" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="F114" s="5"/>
+        <v>131</v>
+      </c>
+      <c r="F114" s="18"/>
       <c r="G114" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="H114" s="5"/>
-    </row>
-    <row r="115" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+      <c r="H114" s="18"/>
+    </row>
+    <row r="115" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A115" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B115" s="6"/>
-      <c r="C115" s="6"/>
-      <c r="D115" s="6"/>
+      <c r="B115" s="18"/>
+      <c r="C115" s="18"/>
+      <c r="D115" s="18"/>
       <c r="E115" s="6">
         <v>75</v>
       </c>
-      <c r="F115" s="6"/>
+      <c r="F115" s="18"/>
       <c r="G115" s="6">
         <v>135</v>
       </c>
-      <c r="H115" s="6"/>
-    </row>
-    <row r="116" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="H115" s="18"/>
+    </row>
+    <row r="116" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A116" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B116" s="6"/>
-      <c r="C116" s="6"/>
-      <c r="D116" s="6"/>
+      <c r="B116" s="18"/>
+      <c r="C116" s="18"/>
+      <c r="D116" s="18"/>
       <c r="E116" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="F116" s="6"/>
+        <v>167</v>
+      </c>
+      <c r="F116" s="18"/>
       <c r="G116" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="H116" s="6"/>
-    </row>
-    <row r="117" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+      <c r="H116" s="18"/>
+    </row>
+    <row r="117" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B117" s="7"/>
-      <c r="C117" s="7"/>
-      <c r="D117" s="7"/>
+      <c r="B117" s="18"/>
+      <c r="C117" s="18"/>
+      <c r="D117" s="18"/>
       <c r="E117" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F117" s="7"/>
+        <v>124</v>
+      </c>
+      <c r="F117" s="18"/>
       <c r="G117" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="H117" s="7"/>
-    </row>
-    <row r="118" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="H117" s="18"/>
+    </row>
+    <row r="118" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B118" s="5"/>
-      <c r="C118" s="5"/>
-      <c r="D118" s="5"/>
+      <c r="B118" s="18"/>
+      <c r="C118" s="18"/>
+      <c r="D118" s="18"/>
       <c r="E118" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="F118" s="5"/>
-      <c r="G118" s="5"/>
-      <c r="H118" s="5"/>
-    </row>
-    <row r="119" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="F118" s="18"/>
+      <c r="G118" s="18"/>
+      <c r="H118" s="18"/>
+    </row>
+    <row r="119" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B119" s="6"/>
-      <c r="C119" s="6"/>
-      <c r="D119" s="6"/>
+      <c r="B119" s="18"/>
+      <c r="C119" s="18"/>
+      <c r="D119" s="18"/>
       <c r="E119" s="6">
         <v>150</v>
       </c>
-      <c r="F119" s="6"/>
-      <c r="G119" s="6"/>
-      <c r="H119" s="6"/>
-    </row>
-    <row r="120" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="F119" s="18"/>
+      <c r="G119" s="18"/>
+      <c r="H119" s="18"/>
+    </row>
+    <row r="120" spans="1:8" ht="15.45" x14ac:dyDescent="0.35">
       <c r="A120" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B120" s="6"/>
-      <c r="C120" s="6"/>
-      <c r="D120" s="6"/>
+      <c r="B120" s="18"/>
+      <c r="C120" s="18"/>
+      <c r="D120" s="18"/>
       <c r="E120" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="F120" s="6"/>
-      <c r="G120" s="6"/>
-      <c r="H120" s="6"/>
-    </row>
-    <row r="121" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+      <c r="F120" s="18"/>
+      <c r="G120" s="18"/>
+      <c r="H120" s="18"/>
+    </row>
+    <row r="121" spans="1:8" ht="28.3" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B121" s="7"/>
-      <c r="C121" s="7"/>
-      <c r="D121" s="7"/>
+      <c r="B121" s="18"/>
+      <c r="C121" s="18"/>
+      <c r="D121" s="18"/>
       <c r="E121" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="F121" s="7"/>
-      <c r="G121" s="7"/>
-      <c r="H121" s="7"/>
+        <v>154</v>
+      </c>
+      <c r="F121" s="18"/>
+      <c r="G121" s="18"/>
+      <c r="H121" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
+  <mergeCells count="18">
     <mergeCell ref="B3:B6"/>
     <mergeCell ref="C3:C6"/>
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="C7:C10"/>
     <mergeCell ref="D7:D10"/>
-    <mergeCell ref="H11:H14"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="C18:C21"/>
     <mergeCell ref="D18:D21"/>
@@ -3563,34 +3550,11 @@
     <mergeCell ref="B11:B14"/>
     <mergeCell ref="C11:C14"/>
     <mergeCell ref="D11:D14"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="G11:G14"/>
     <mergeCell ref="C26:C29"/>
     <mergeCell ref="D26:D29"/>
     <mergeCell ref="C22:C25"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
-    <mergeCell ref="F26:F29"/>
-    <mergeCell ref="G26:G29"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="G33:G36"/>
-    <mergeCell ref="G37:G40"/>
-    <mergeCell ref="G41:G44"/>
-    <mergeCell ref="B41:B44"/>
-    <mergeCell ref="C41:C44"/>
-    <mergeCell ref="D41:D44"/>
-    <mergeCell ref="E41:E44"/>
-    <mergeCell ref="F41:F44"/>
-    <mergeCell ref="H56:H59"/>
-    <mergeCell ref="H60:H63"/>
-    <mergeCell ref="G60:G63"/>
-    <mergeCell ref="B56:B59"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="D56:D59"/>
-    <mergeCell ref="E60:E63"/>
-    <mergeCell ref="D60:D63"/>
-    <mergeCell ref="C60:C63"/>
-    <mergeCell ref="B60:B63"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>